<commit_message>
this is 25 jan
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>jdhajh</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>dskjha</t>
+  </si>
+  <si>
+    <t>djhfjh</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
@@ -416,6 +419,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
this is new one
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -48,7 +48,7 @@
     <t>dskjha</t>
   </si>
   <si>
-    <t>djhfjh</t>
+    <t>djfkj</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>